<commit_message>
use excel input to control which rbd is round trip only
</commit_message>
<xml_diff>
--- a/python/fare-filing/gg_fare_filing.xlsx
+++ b/python/fare-filing/gg_fare_filing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="57480" yWindow="7455" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="57480" yWindow="7455" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" state="visible" r:id="rId1"/>
@@ -210,18 +210,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
     <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
@@ -245,6 +245,9 @@
         <vertAlign val="baseline"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
@@ -371,26 +374,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:F71" headerRowCount="1" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:F71" headerRowCount="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:F71"/>
   <tableColumns count="6">
-    <tableColumn id="6" name="sort" dataDxfId="20"/>
-    <tableColumn id="1" name="dest" dataDxfId="19"/>
-    <tableColumn id="2" name="booking_class" dataDxfId="18"/>
-    <tableColumn id="3" name="season" dataDxfId="17"/>
-    <tableColumn id="4" name="base_fare" dataDxfId="16"/>
-    <tableColumn id="5" name="direct" dataDxfId="15"/>
+    <tableColumn id="6" name="sort" dataDxfId="21"/>
+    <tableColumn id="1" name="dest" dataDxfId="20"/>
+    <tableColumn id="2" name="booking_class" dataDxfId="19"/>
+    <tableColumn id="3" name="season" dataDxfId="18"/>
+    <tableColumn id="4" name="base_fare" dataDxfId="17"/>
+    <tableColumn id="5" name="direct" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B18" headerRowCount="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="booking_class" dataDxfId="12"/>
-    <tableColumn id="2" name="cabin" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C18" headerRowCount="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:C18"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="booking_class" dataDxfId="13"/>
+    <tableColumn id="2" name="cabin" dataDxfId="12"/>
+    <tableColumn id="3" name="rt_only" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -412,9 +416,9 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="weekend" dataDxfId="4"/>
-    <tableColumn id="2" name="weekend_surcharge" dataDxfId="3"/>
-    <tableColumn id="3" name="oneway" dataDxfId="2"/>
-    <tableColumn id="4" name="oneway_multiplier" dataDxfId="1"/>
+    <tableColumn id="4" name="oneway_multiplier" dataDxfId="3"/>
+    <tableColumn id="2" name="weekend_surcharge" dataDxfId="2"/>
+    <tableColumn id="3" name="oneway" dataDxfId="1"/>
     <tableColumn id="5" name="oneway_mapping" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -730,15 +734,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="9.109375" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="16.44140625" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
-    <col width="11.21875" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="13.77734375" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="10.33203125" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
-    <col width="8.77734375" customWidth="1" style="9" min="6" max="7"/>
+    <col width="8.77734375" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
+    <col width="9.109375" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="10.44140625" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
+    <col width="8.77734375" customWidth="1" style="9" min="7" max="7"/>
     <col width="15.6640625" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
-    <col width="8.77734375" customWidth="1" style="9" min="9" max="27"/>
-    <col width="8.77734375" customWidth="1" style="9" min="28" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="9" min="9" max="31"/>
+    <col width="8.77734375" customWidth="1" style="9" min="32" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1086,16 +1091,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="17.21875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="17.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.5546875" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1109,6 +1115,11 @@
           <t>cabin</t>
         </is>
       </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>rt_only</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="inlineStr">
@@ -1121,6 +1132,7 @@
           <t>Premium Economy</t>
         </is>
       </c>
+      <c r="C2" s="9" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
@@ -1133,6 +1145,7 @@
           <t>Premium Economy</t>
         </is>
       </c>
+      <c r="C3" s="9" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="inlineStr">
@@ -1145,6 +1158,7 @@
           <t>Premium Economy</t>
         </is>
       </c>
+      <c r="C4" s="9" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
@@ -1157,6 +1171,7 @@
           <t>Premium Economy</t>
         </is>
       </c>
+      <c r="C5" s="9" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="inlineStr">
@@ -1169,6 +1184,11 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="inlineStr">
@@ -1181,6 +1201,11 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
@@ -1193,6 +1218,11 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C8" s="9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
@@ -1205,6 +1235,11 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="inlineStr">
@@ -1217,6 +1252,7 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C10" s="9" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="9" t="inlineStr">
@@ -1229,6 +1265,7 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C11" s="9" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="inlineStr">
@@ -1241,6 +1278,11 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="inlineStr">
@@ -1253,6 +1295,7 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C13" s="9" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
@@ -1265,6 +1308,7 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C14" s="9" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="inlineStr">
@@ -1277,6 +1321,7 @@
           <t>Economy</t>
         </is>
       </c>
+      <c r="C15" s="9" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="9" t="inlineStr">
@@ -1289,6 +1334,7 @@
           <t>Business</t>
         </is>
       </c>
+      <c r="C16" s="9" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="9" t="inlineStr">
@@ -1301,6 +1347,7 @@
           <t>Business</t>
         </is>
       </c>
+      <c r="C17" s="9" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="9" t="inlineStr">
@@ -1313,6 +1360,7 @@
           <t>Business</t>
         </is>
       </c>
+      <c r="C18" s="9" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1472,19 +1520,19 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col width="13.33203125" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="22.77734375" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
-    <col width="12.109375" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="21.77734375" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="20.5546875" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
-    <col width="8.77734375" customWidth="1" style="9" min="6" max="29"/>
-    <col width="8.77734375" customWidth="1" style="9" min="30" max="16384"/>
+    <col width="21.77734375" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
+    <col width="22.77734375" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="12.109375" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
+    <col width="20.5546875" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
+    <col width="8.77734375" customWidth="1" style="9" min="7" max="34"/>
+    <col width="8.77734375" customWidth="1" style="9" min="35" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1495,17 +1543,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>oneway_multiplier</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>weekend_surcharge</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>oneway</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>oneway_multiplier</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -1520,11 +1568,11 @@
           <t>X</t>
         </is>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="n">
         <v>0</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1</v>
       </c>
       <c r="E2" s="9" t="inlineStr">
         <is>
@@ -1538,11 +1586,11 @@
           <t>X</t>
         </is>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="n">
         <v>80</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>1</v>
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
@@ -1556,11 +1604,16 @@
           <t>W</t>
         </is>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="2" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>0.65</v>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
@@ -1574,11 +1627,16 @@
           <t>W</t>
         </is>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="2" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C5" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>0.65</v>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
@@ -1678,7 +1736,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JLXSE</t>
+          <t>JLXUS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1721,7 +1779,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JLXSE</t>
+          <t>JLXUS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1764,7 +1822,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JLWSE</t>
+          <t>JLWOUS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1807,7 +1865,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>JLWSE</t>
+          <t>JLWOUS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1850,7 +1908,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CLXSE</t>
+          <t>CLXUS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1893,7 +1951,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CLXSE</t>
+          <t>CLXUS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1936,7 +1994,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CLWSE</t>
+          <t>CLWOUS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1979,7 +2037,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CLWSE</t>
+          <t>CLWOUS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2022,7 +2080,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DLXSE</t>
+          <t>DLXUS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2065,7 +2123,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DLXSE</t>
+          <t>DLXUS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2108,7 +2166,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DLWSE</t>
+          <t>DLWOUS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2151,7 +2209,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DLWSE</t>
+          <t>DLWOUS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2270,7 +2328,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JK1XSE</t>
+          <t>JKXUS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2313,7 +2371,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JK1XSE</t>
+          <t>JKXUS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2356,7 +2414,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JK1WSE</t>
+          <t>JKWOUS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2399,7 +2457,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>JK1WSE</t>
+          <t>JKWOUS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2442,7 +2500,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CK1XSE</t>
+          <t>CKXUS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2485,7 +2543,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CK1XSE</t>
+          <t>CKXUS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2528,7 +2586,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CK1WSE</t>
+          <t>CKWOUS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2571,7 +2629,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CK1WSE</t>
+          <t>CKWOUS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2614,7 +2672,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DK1XSE</t>
+          <t>DKXUS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2657,7 +2715,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DK1XSE</t>
+          <t>DKXUS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2700,7 +2758,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DK1WSE</t>
+          <t>DKWOUS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2743,7 +2801,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DK1WSE</t>
+          <t>DKWOUS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2862,7 +2920,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JH1XSE</t>
+          <t>JHXUS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2905,7 +2963,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JH1XSE</t>
+          <t>JHXUS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2948,7 +3006,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JH1WSE</t>
+          <t>JHWOUS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2991,7 +3049,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>JH1WSE</t>
+          <t>JHWOUS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3034,7 +3092,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CH1XSE</t>
+          <t>CHXUS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3077,7 +3135,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CH1XSE</t>
+          <t>CHXUS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3120,7 +3178,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CH1WSE</t>
+          <t>CHWOUS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3163,7 +3221,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CH1WSE</t>
+          <t>CHWOUS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3206,7 +3264,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DH1XSE</t>
+          <t>DHXUS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3249,7 +3307,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DH1XSE</t>
+          <t>DHXUS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3292,7 +3350,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DH1WSE</t>
+          <t>DHWOUS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3335,7 +3393,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DH1WSE</t>
+          <t>DHWOUS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3454,7 +3512,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JPXSE</t>
+          <t>JPXUS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3497,7 +3555,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>JPXSE</t>
+          <t>JPXUS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3540,7 +3598,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JPWSE</t>
+          <t>JPWOUS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3583,7 +3641,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>JPWSE</t>
+          <t>JPWOUS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3626,7 +3684,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CPXSE</t>
+          <t>CPXUS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3669,7 +3727,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CPXSE</t>
+          <t>CPXUS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3712,7 +3770,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CPWSE</t>
+          <t>CPWOUS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3755,7 +3813,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CPWSE</t>
+          <t>CPWOUS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3798,7 +3856,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DPXSE</t>
+          <t>DPXUS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3841,7 +3899,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DPXSE</t>
+          <t>DPXUS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3884,7 +3942,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DPWSE</t>
+          <t>DPWOUS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3927,7 +3985,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DPWSE</t>
+          <t>DPWOUS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">

</xml_diff>